<commit_message>
Updated calculator for Lily
</commit_message>
<xml_diff>
--- a/Flower bots/Lily/Calculator Lily materials.xlsx
+++ b/Flower bots/Lily/Calculator Lily materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rosehulman-my.sharepoint.com/personal/marcena_rose-hulman_edu/Documents/Robotics research/Flower bots/Lily/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcena\Documents\GitHub\Lily-Bot\Flower bots\Lily\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{7A3E8E9A-D8AC-4E92-83BF-CE9458B6F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F6BD7D-0C8D-46F9-A9A7-30781937D17E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6173A6FE-32E5-4632-A9B6-19C455B1BB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8A1122B-ACA5-4C8A-9434-2F2872F05A91}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Need</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Total material (g)</t>
+  </si>
+  <si>
+    <t>Motor mount</t>
+  </si>
+  <si>
+    <t>Motor controller</t>
+  </si>
+  <si>
+    <t>IR/photoresistor mounts</t>
   </si>
 </sst>
 </file>
@@ -161,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +195,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -603,21 +618,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -627,92 +783,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -720,37 +792,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1213,18 +1276,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F805AB76-66CA-4BC0-97CF-73CC4FEA8C41}">
-  <dimension ref="B2:N29"/>
+  <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
@@ -1233,11 +1296,11 @@
   <sheetData>
     <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2">
-        <v>36</v>
+      <c r="C3" s="46">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
@@ -1247,519 +1310,518 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="46" t="s">
+      <c r="I7" s="30"/>
+      <c r="J7" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="42" t="s">
+      <c r="M7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="43" t="s">
+      <c r="N7" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="13">
-        <f t="shared" ref="E8:E14" si="0">G8-F8</f>
-        <v>28</v>
-      </c>
-      <c r="F8" s="14">
+      <c r="E8" s="9">
+        <f>IF(G8-F8&gt;0,G8-F8,0)</f>
+        <v>16</v>
+      </c>
+      <c r="F8" s="47"/>
+      <c r="G8" s="10">
+        <f>$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="34">
+        <v>3.5</v>
+      </c>
+      <c r="L8" s="28">
+        <f>K8*$E8</f>
+        <v>56</v>
+      </c>
+      <c r="M8" s="28">
+        <v>37.36</v>
+      </c>
+      <c r="N8" s="29">
+        <f>M8*$E8</f>
+        <v>597.76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="39"/>
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="12">
+        <f>IF(G9-F9&gt;0,G9-F9,0)</f>
+        <v>16</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="13">
+        <f t="shared" ref="G9:G11" si="0">$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="I9" s="42"/>
+      <c r="J9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="24">
+        <f t="shared" ref="L9:N11" si="1">K9*E9</f>
+        <v>24</v>
+      </c>
+      <c r="M9" s="24">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="N9" s="27">
+        <f>M9*G9</f>
+        <v>259.04000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C10" s="39"/>
+      <c r="D10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" ref="E10:E30" si="2">IF(G10-F10&gt;0,G10-F10,0)</f>
+        <v>16</v>
+      </c>
+      <c r="F10" s="48"/>
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="I10" s="42"/>
+      <c r="J10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="23">
+        <v>5</v>
+      </c>
+      <c r="L10" s="24">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="M10" s="24">
+        <v>53.36</v>
+      </c>
+      <c r="N10" s="27">
+        <f t="shared" si="1"/>
+        <v>853.76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C11" s="39"/>
+      <c r="D11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F11" s="48"/>
+      <c r="G11" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="I11" s="42"/>
+      <c r="J11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="23">
+        <v>1.33</v>
+      </c>
+      <c r="L11" s="24">
+        <f t="shared" si="1"/>
+        <v>21.28</v>
+      </c>
+      <c r="M11" s="24">
+        <v>16.48</v>
+      </c>
+      <c r="N11" s="27">
+        <f t="shared" si="1"/>
+        <v>263.68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="39"/>
+      <c r="D12" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F12" s="49"/>
+      <c r="G12" s="45">
+        <f>C3*2</f>
+        <v>32</v>
+      </c>
+      <c r="I12" s="42"/>
+      <c r="J12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="27"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C13" s="39"/>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="12">
+        <f>IF(G13-F13&gt;0,G13-F13,0)</f>
+        <v>16</v>
+      </c>
+      <c r="F13" s="48"/>
+      <c r="G13" s="13">
+        <f t="shared" ref="G13:G18" si="3">$C$3</f>
+        <v>16</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="J13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="27"/>
+    </row>
+    <row r="14" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C14" s="39"/>
+      <c r="D14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="13">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I14" s="42"/>
+      <c r="J14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="27"/>
+    </row>
+    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="40"/>
+      <c r="D15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="15">
-        <f>$C$3</f>
-        <v>36</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="45">
-        <v>3.5</v>
-      </c>
-      <c r="L8" s="39">
-        <f>K8*$E8</f>
-        <v>98</v>
-      </c>
-      <c r="M8" s="39">
-        <v>37.36</v>
-      </c>
-      <c r="N8" s="40">
-        <f>M8*$E8</f>
-        <v>1046.08</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
-      <c r="D9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="17">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="F9" s="18">
+      <c r="E15" s="15">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="G15" s="16">
+        <f>$C$3*4</f>
+        <v>64</v>
+      </c>
+      <c r="I15" s="42"/>
+      <c r="J15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0.433</v>
+      </c>
+      <c r="L15" s="24">
+        <f>IF(E15&gt;0,K15*E15,0)</f>
+        <v>27.712</v>
+      </c>
+      <c r="M15" s="24">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="N15" s="27">
+        <f>M15*G15</f>
+        <v>146.49600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="19">
-        <f t="shared" ref="G9:G11" si="1">$C$3</f>
-        <v>36</v>
-      </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="L9" s="32">
-        <f t="shared" ref="L9:N12" si="2">K9*E9</f>
-        <v>40.5</v>
-      </c>
-      <c r="M9" s="32">
-        <v>16.190000000000001</v>
-      </c>
-      <c r="N9" s="35">
-        <f>M9*G9</f>
-        <v>582.84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
-      <c r="D10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="17">
-        <f t="shared" si="0"/>
+      <c r="D16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="19">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="31">
-        <v>5</v>
-      </c>
-      <c r="L10" s="32">
+      <c r="E16" s="18">
         <f t="shared" si="2"/>
-        <v>175</v>
-      </c>
-      <c r="M10" s="32">
-        <v>53.36</v>
-      </c>
-      <c r="N10" s="35">
+        <v>32</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="19">
+        <f>$C$3*2</f>
+        <v>32</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="J16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="26">
+        <f>SUM(L8:L15)</f>
+        <v>208.99199999999999</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="37">
+        <f>SUM(N8:N15)</f>
+        <v>2120.7359999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="39"/>
+      <c r="D17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="12">
         <f t="shared" si="2"/>
-        <v>1920.96</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="5"/>
-      <c r="D11" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="17">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="F11" s="18">
-        <v>3</v>
-      </c>
-      <c r="G11" s="19">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="31">
-        <v>1.33</v>
-      </c>
-      <c r="L11" s="32">
+        <v>16</v>
+      </c>
+      <c r="F17" s="48"/>
+      <c r="G17" s="13">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="39"/>
+      <c r="D18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="12">
         <f t="shared" si="2"/>
-        <v>43.89</v>
-      </c>
-      <c r="M11" s="32">
-        <v>16.48</v>
-      </c>
-      <c r="N11" s="35">
+        <v>16</v>
+      </c>
+      <c r="F18" s="48"/>
+      <c r="G18" s="13">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="39"/>
+      <c r="D19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="12">
         <f t="shared" si="2"/>
-        <v>593.28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="6"/>
-      <c r="D12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="21">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="F12" s="22">
-        <v>75</v>
-      </c>
-      <c r="G12" s="23">
+        <v>32</v>
+      </c>
+      <c r="F19" s="48"/>
+      <c r="G19" s="13">
+        <f t="shared" ref="G19:G22" si="4">$C$3*2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="39"/>
+      <c r="D20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F20" s="48"/>
+      <c r="G20" s="13">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C21" s="39"/>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F21" s="48"/>
+      <c r="G21" s="13">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="39"/>
+      <c r="D22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="12">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="F22" s="48"/>
+      <c r="G22" s="13">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="39"/>
+      <c r="D23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="12">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F23" s="48"/>
+      <c r="G23" s="13">
+        <f t="shared" ref="G23:G24" si="5">$C$3</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="39"/>
+      <c r="D24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="12">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F24" s="48"/>
+      <c r="G24" s="13">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="39"/>
+      <c r="D25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="48"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="39"/>
+      <c r="D26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="48"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="39"/>
+      <c r="D27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="12">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F27" s="48"/>
+      <c r="G27" s="13">
         <f>$C$3*4</f>
-        <v>144</v>
-      </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="31">
-        <v>0.433</v>
-      </c>
-      <c r="L12" s="32">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C28" s="39"/>
+      <c r="D28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="12">
         <f t="shared" si="2"/>
-        <v>29.876999999999999</v>
-      </c>
-      <c r="M12" s="32">
-        <v>2.2890000000000001</v>
-      </c>
-      <c r="N12" s="35">
+        <v>64</v>
+      </c>
+      <c r="F28" s="48"/>
+      <c r="G28" s="13">
+        <f>$C$3*4</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C29" s="39"/>
+      <c r="D29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="12">
         <f t="shared" si="2"/>
-        <v>329.61600000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="25">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="F13" s="26">
-        <v>2</v>
-      </c>
-      <c r="G13" s="27">
-        <f>$C$3*2</f>
-        <v>72</v>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="34">
-        <f>SUM(L8:L12)</f>
-        <v>387.267</v>
-      </c>
-      <c r="M13" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="48">
-        <f>SUM(N8:N12)</f>
-        <v>4472.7759999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="17">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0</v>
-      </c>
-      <c r="G14" s="19">
-        <f t="shared" ref="G14:G17" si="3">$C$3</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
-      <c r="D15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="17">
-        <f>G15-F15</f>
-        <v>6</v>
-      </c>
-      <c r="F15" s="18">
-        <v>30</v>
-      </c>
-      <c r="G15" s="19">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="17">
-        <f>G16-F16</f>
-        <v>27</v>
-      </c>
-      <c r="F16" s="18">
-        <v>9</v>
-      </c>
-      <c r="G16" s="19">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C17" s="5"/>
-      <c r="D17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="17">
-        <f t="shared" ref="E17:E29" si="4">G17-F17</f>
-        <v>9</v>
-      </c>
-      <c r="F17" s="18">
-        <v>27</v>
-      </c>
-      <c r="G17" s="19">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C18" s="5"/>
-      <c r="D18" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="17">
-        <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="F18" s="18">
-        <v>23</v>
-      </c>
-      <c r="G18" s="19">
-        <f t="shared" ref="G18:G21" si="5">$C$3*2</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="5"/>
-      <c r="D19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="17">
-        <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="F19" s="18">
-        <v>20</v>
-      </c>
-      <c r="G19" s="19">
-        <f t="shared" si="5"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="5"/>
-      <c r="D20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="17">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-      <c r="F20" s="18">
-        <v>21</v>
-      </c>
-      <c r="G20" s="19">
-        <f t="shared" si="5"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="5"/>
-      <c r="D21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="17">
-        <f t="shared" si="4"/>
-        <v>53</v>
-      </c>
-      <c r="F21" s="18">
-        <v>19</v>
-      </c>
-      <c r="G21" s="19">
-        <f t="shared" si="5"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
-      <c r="D22" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="17">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="F22" s="18">
+        <v>16</v>
+      </c>
+      <c r="F29" s="48"/>
+      <c r="G29" s="13">
+        <f t="shared" ref="G29:G30" si="6">$C$3</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="40"/>
+      <c r="D30" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="19">
-        <f t="shared" ref="G22:G23" si="6">$C$3</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="5"/>
-      <c r="D23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="17">
-        <f t="shared" si="4"/>
-        <v>34</v>
-      </c>
-      <c r="F23" s="18">
-        <v>2</v>
-      </c>
-      <c r="G23" s="19">
+      <c r="E30" s="15">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F30" s="50"/>
+      <c r="G30" s="16">
         <f t="shared" si="6"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
-      <c r="D24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="5"/>
-      <c r="D25" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="5"/>
-      <c r="D26" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>144</v>
-      </c>
-      <c r="G26" s="19">
-        <f>$C$3*4</f>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="5"/>
-      <c r="D27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>144</v>
-      </c>
-      <c r="G27" s="19">
-        <f>$C$3*4</f>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="5"/>
-      <c r="D28" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>36</v>
-      </c>
-      <c r="G28" s="19">
-        <f t="shared" ref="G28:G29" si="7">$C$3</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="6"/>
-      <c r="D29" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="22">
-        <v>36</v>
-      </c>
-      <c r="G29" s="23">
-        <f t="shared" si="7"/>
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="C16:C30"/>
+    <mergeCell ref="I8:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>